<commit_message>
Updates to styles and data
</commit_message>
<xml_diff>
--- a/KFLA/Data/data.en.xlsx
+++ b/KFLA/Data/data.en.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="545">
   <si>
     <t xml:space="preserve">Comp #</t>
   </si>
@@ -2579,6 +2579,42 @@
   </si>
   <si>
     <t xml:space="preserve">No competencies evaluated. Redirrecting...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.Scales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competency rating scales </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.PossibleCauses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible causes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.Tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tips to develop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.Reflect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to reflect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library.Items.Links.LearnMore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn more</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -2823,7 +2859,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2900,10 +2936,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2921,6 +2953,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2956,7 +3000,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="49.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="72.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="3" width="26.85"/>
@@ -4527,14 +4571,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="39.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="17" width="57.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -4548,39 +4592,39 @@
       <c r="C1" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>383</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>386</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="n">
+      <c r="A2" s="20" t="n">
         <v>101</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>389</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>391</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -4597,19 +4641,19 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="212.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
+      <c r="A3" s="20" t="n">
         <v>102</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>389</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>398</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -4624,19 +4668,19 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="n">
+      <c r="A4" s="20" t="n">
         <v>103</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>402</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>389</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>404</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -4649,19 +4693,19 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="171.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="20" t="n">
         <v>104</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>410</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -4678,19 +4722,19 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="140.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="n">
+      <c r="A6" s="20" t="n">
         <v>105</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>417</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -4705,19 +4749,19 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="n">
+      <c r="A7" s="20" t="n">
         <v>106</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>423</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -4728,19 +4772,19 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="n">
+      <c r="A8" s="20" t="n">
         <v>107</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>428</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -4753,19 +4797,19 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="156" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="n">
+      <c r="A9" s="20" t="n">
         <v>108</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>431</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>433</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -4780,19 +4824,19 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="n">
+      <c r="A10" s="20" t="n">
         <v>109</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>438</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>439</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -4803,19 +4847,19 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="186.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+      <c r="A11" s="20" t="n">
         <v>110</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>443</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -4843,15 +4887,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
@@ -5176,6 +5220,59 @@
         <v>4</v>
       </c>
     </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="24" t="s">
+        <v>516</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="24" t="s">
+        <v>526</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="24"/>
+      <c r="B47" s="26"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5211,22 +5308,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>380</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,19 +5331,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5254,19 +5351,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5274,19 +5371,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>